<commit_message>
Completed first draft of results.
Completed text of draft results section. Implemented fixes and adjustments following discussion at the 20220517 meeting. Remade tables of crude results with incidence rate ratios and confidence intervals. Added cleaned up ANOVA tables of O/O and O models. Assigned prettier names to files with tables and figures.
</commit_message>
<xml_diff>
--- a/output/table2.xlsx
+++ b/output/table2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Intact, n = 109,467</t>
   </si>
@@ -25,28 +25,31 @@
     <t>Overweight/obese</t>
   </si>
   <si>
+    <t>Outcome events, n</t>
+  </si>
+  <si>
     <t>Total years of observation</t>
   </si>
   <si>
-    <t>Crude outcome events, n (%)</t>
-  </si>
-  <si>
-    <t>24,405 (22.3)</t>
-  </si>
-  <si>
-    <t>17,852 (39.0)</t>
-  </si>
-  <si>
-    <t>Crude outcome incidence rates per 1,000 years of observation</t>
+    <t>Crude incidence rates per 1,000 years of observation</t>
+  </si>
+  <si>
+    <t>Crude incidence rate ratio (95% CI)</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>1.91 (1.87, 1.95)</t>
   </si>
   <si>
     <t>Obese</t>
   </si>
   <si>
-    <t>1,208 (1.1)</t>
-  </si>
-  <si>
-    <t>1,920 (4.2)</t>
+    <t>Outcome events, n (%)</t>
+  </si>
+  <si>
+    <t>3.49 (3.25, 3.75)</t>
   </si>
 </sst>
 </file>
@@ -531,13 +534,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -875,110 +877,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>248109</v>
-      </c>
-      <c r="C3" s="1">
-        <v>95039</v>
+      <c r="B3" s="2">
+        <v>24405</v>
+      </c>
+      <c r="C3" s="2">
+        <v>17852</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
+      <c r="B4" s="2">
+        <v>248109</v>
+      </c>
+      <c r="C4" s="2">
+        <v>95039</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
         <v>98.4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>187.8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>289543</v>
-      </c>
-      <c r="C7" s="1">
-        <v>131839</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1208</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1920</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>289543</v>
+      </c>
+      <c r="C9" s="2">
+        <v>131839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>4.2</v>
-      </c>
-      <c r="C9">
-        <v>14.6</v>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A6:C6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>